<commit_message>
testing if i can push this new test.txt file
</commit_message>
<xml_diff>
--- a/sql/Lab1-3/Week2_Lab1-3_sql.xlsx
+++ b/sql/Lab1-3/Week2_Lab1-3_sql.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinacastillo/Desktop/DS311/sql/Lab1-3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christinacastillo/Desktop/SQL_HW/sql/Lab1-3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A5BB55-787B-4243-8A19-46E1DD1676BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285D599F-C451-6D4E-8F74-73A7469C3A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49880" yWindow="10500" windowWidth="46360" windowHeight="10520" firstSheet="5" activeTab="14" xr2:uid="{4F2F94B7-517C-3646-B85E-AF7D05656805}"/>
+    <workbookView xWindow="-46320" yWindow="10500" windowWidth="46320" windowHeight="10520" xr2:uid="{4F2F94B7-517C-3646-B85E-AF7D05656805}"/>
   </bookViews>
   <sheets>
     <sheet name="L1P1q1" sheetId="1" r:id="rId1"/>
@@ -2145,8 +2145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{397F3237-EFD7-1547-8DC0-7AC117BFFCDE}">
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="25.33203125" defaultRowHeight="27" x14ac:dyDescent="0.35"/>
@@ -5013,10 +5013,13 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CF37671-EB85-4240-8BA4-BBCA6993A6AB}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5060,10 +5063,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F84265C6-E5C8-7F46-B7DA-03B798E5D747}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5120,10 +5126,13 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B47B60C-FDA8-2B4C-9F75-D2179B64124E}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5178,10 +5187,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F0A63E6-D055-4B47-A16A-C0218F8181B9}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D7"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5291,10 +5303,13 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1000EC11-799F-5841-B770-804D03211F05}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G2"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5352,10 +5367,13 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20A90698-F0D1-2A47-8677-2606074E1B0F}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G4"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5628,10 +5646,13 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D14B6090-3CBB-E742-8ED8-5D2C6E52D617}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5691,10 +5712,13 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68538E35-8753-0A46-9046-E2C805B3D6B3}">
+  <sheetPr>
+    <tabColor theme="2"/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C7"/>
+      <selection activeCell="Y14" sqref="Y14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>